<commit_message>
add new test with business API
</commit_message>
<xml_diff>
--- a/quarkus/src/test/resources/KYC.xlsx
+++ b/quarkus/src/test/resources/KYC.xlsx
@@ -26,7 +26,7 @@
     <author>Greg Autric</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -35,12 +35,11 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">@input
-</t>
+          <t>@input(PEP)</t>
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,12 +48,12 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">@input
+          <t xml:space="preserve">@input(COUNTRY)
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +62,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">@input
+          <t xml:space="preserve">@input(AMOUNT)
 </t>
         </r>
       </text>
@@ -77,7 +76,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">@output
+          <t xml:space="preserve">@output(SCORE)
 </t>
         </r>
       </text>
@@ -540,7 +539,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>